<commit_message>
updated knight and archer unit xls
Added new directory and obstacles.psd
</commit_message>
<xml_diff>
--- a/assets/Archer/Archer Unit Sprite Notes.xlsx
+++ b/assets/Archer/Archer Unit Sprite Notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="25">
   <si>
     <t>Action</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Dead</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>96X96</t>
   </si>
 </sst>
 </file>
@@ -440,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="B23:D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -449,6 +455,7 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
@@ -467,6 +474,9 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10">
@@ -481,6 +491,9 @@
       </c>
       <c r="D3">
         <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -497,6 +510,9 @@
       <c r="D4">
         <v>9</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -512,6 +528,9 @@
       <c r="D5">
         <v>9</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
@@ -527,6 +546,9 @@
       <c r="D6">
         <v>9</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
@@ -542,6 +564,9 @@
       <c r="D7" s="1">
         <v>9</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="H7" t="s">
         <v>16</v>
       </c>
@@ -566,6 +591,9 @@
       <c r="D8" s="1">
         <v>9</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:10">
@@ -582,6 +610,9 @@
       <c r="D9" s="1">
         <v>9</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
@@ -603,6 +634,9 @@
       <c r="D10" s="1">
         <v>9</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
@@ -618,6 +652,9 @@
       <c r="D11">
         <v>13</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="H11" t="s">
         <v>19</v>
       </c>
@@ -642,6 +679,9 @@
       <c r="D12">
         <v>13</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
@@ -657,6 +697,9 @@
       <c r="D13">
         <v>13</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
@@ -672,6 +715,9 @@
       <c r="D14">
         <v>13</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
@@ -687,6 +733,9 @@
       <c r="D15" s="1">
         <v>8</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
@@ -702,8 +751,11 @@
       <c r="D16" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="F16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -717,8 +769,11 @@
       <c r="D17" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -732,8 +787,11 @@
       <c r="D18" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="F18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -747,8 +805,11 @@
       <c r="D19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -762,8 +823,11 @@
       <c r="D20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -777,8 +841,11 @@
       <c r="D21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="F21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -792,8 +859,11 @@
       <c r="D22">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -807,8 +877,11 @@
       <c r="D23" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -822,8 +895,11 @@
       <c r="D24" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -837,8 +913,11 @@
       <c r="D25" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -852,8 +931,11 @@
       <c r="D26" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -864,8 +946,11 @@
       <c r="D27">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -876,8 +961,11 @@
       <c r="D28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="F28" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -888,8 +976,11 @@
       <c r="D29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="F29" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -900,8 +991,11 @@
       <c r="D30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="F30" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -912,8 +1006,11 @@
       <c r="D31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="F31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -924,8 +1021,11 @@
       <c r="D32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="F32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -936,8 +1036,11 @@
       <c r="D33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="F33" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -948,8 +1051,11 @@
       <c r="D34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -960,8 +1066,11 @@
       <c r="D35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="F35" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -972,8 +1081,11 @@
       <c r="D36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="F36" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -984,8 +1096,11 @@
       <c r="D37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="F37" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -996,8 +1111,11 @@
       <c r="D38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="F38" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1008,8 +1126,11 @@
       <c r="D39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="F39" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1020,8 +1141,11 @@
       <c r="D40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="F40" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1032,8 +1156,11 @@
       <c r="D41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="F41" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1044,8 +1171,11 @@
       <c r="D42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="F42" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1056,8 +1186,11 @@
       <c r="D43">
         <v>13</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="F43" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1068,8 +1201,11 @@
       <c r="D44">
         <v>13</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="F44" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1080,8 +1216,11 @@
       <c r="D45">
         <v>13</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="F45" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1092,8 +1231,11 @@
       <c r="D46">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="F46" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1104,8 +1246,11 @@
       <c r="D47">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="F47" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1116,8 +1261,11 @@
       <c r="D48">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="F48" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1128,8 +1276,11 @@
       <c r="D49">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="F49" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1139,6 +1290,9 @@
       </c>
       <c r="D50">
         <v>13</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>